<commit_message>
Small tasks and updates
</commit_message>
<xml_diff>
--- a/Task2/Diversification-Tool.xlsx
+++ b/Task2/Diversification-Tool.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\npric\Desktop\Melbourne University\2018\Algorithmic Trading\FNCE30010Project1\Task2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81950959-68A7-448F-926C-E1EBBE7E6019}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4A7AC77-3850-4EB3-B1C9-441366E75235}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Diversification" sheetId="1" r:id="rId1"/>
@@ -652,17 +652,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA25"/>
+  <dimension ref="A1:Y25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Z12" sqref="Z12"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="11" width="10.6640625" style="3"/>
     <col min="12" max="12" width="11.44140625" style="3" customWidth="1"/>
-    <col min="13" max="26" width="10.6640625" style="3" customWidth="1"/>
+    <col min="13" max="14" width="10.6640625" style="3" customWidth="1"/>
+    <col min="15" max="15" width="12.5546875" style="3" customWidth="1"/>
+    <col min="16" max="16" width="20.5546875" style="3" customWidth="1"/>
+    <col min="17" max="18" width="10.6640625" style="3" customWidth="1"/>
+    <col min="19" max="19" width="14.21875" style="3" customWidth="1"/>
+    <col min="20" max="20" width="10.6640625" style="3" customWidth="1"/>
+    <col min="21" max="21" width="17.77734375" style="3" customWidth="1"/>
+    <col min="22" max="26" width="10.6640625" style="3" customWidth="1"/>
     <col min="27" max="27" width="22" style="3" customWidth="1"/>
     <col min="28" max="16384" width="10.6640625" style="3"/>
   </cols>

</xml_diff>